<commit_message>
Added the final analiza_testiranja.docx
</commit_message>
<xml_diff>
--- a/analiza_uporabniskega_AB_testiranja.xlsx
+++ b/analiza_uporabniskega_AB_testiranja.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\KCR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KCR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD94FADC-9651-4BFC-A18E-5761B545D5E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4F3940-AA46-489B-95B2-EDD83A629090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3465" yWindow="2895" windowWidth="25335" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1433,8 +1433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BD53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="U13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y18" sqref="Y18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4014,7 +4014,7 @@
       </c>
       <c r="U22" s="2"/>
       <c r="V22" s="5"/>
-      <c r="W22" s="2" t="s">
+      <c r="W22" s="5" t="s">
         <v>193</v>
       </c>
       <c r="X22" s="5">

</xml_diff>

<commit_message>
Updates readme, fixes typos in files
</commit_message>
<xml_diff>
--- a/analiza_uporabniskega_AB_testiranja.xlsx
+++ b/analiza_uporabniskega_AB_testiranja.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KCR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anapoklukar/Desktop/kcr_project/KCR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4F3940-AA46-489B-95B2-EDD83A629090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE16623-619F-AC4B-880C-5AFF6FE3E6C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="2895" windowWidth="25335" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="194">
   <si>
     <t>test 1</t>
   </si>
@@ -125,9 +125,6 @@
     <t>splet</t>
   </si>
   <si>
-    <t>9.12.24, 20.36</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -233,9 +230,6 @@
     <t>živo</t>
   </si>
   <si>
-    <t>10. 12. 2024, 9.30</t>
-  </si>
-  <si>
     <t>Rabu ful časa na first pagu, skrit gumb, vizualna hierarhija ni najboljsa, je samoumevn</t>
   </si>
   <si>
@@ -279,9 +273,6 @@
   </si>
   <si>
     <t>Ja, razvija podobno, ne čisto</t>
-  </si>
-  <si>
-    <t>10. 12. 2024, 9.50</t>
   </si>
   <si>
     <t>B</t>
@@ -364,9 +355,6 @@
   </si>
   <si>
     <t>Ne nikoli</t>
-  </si>
-  <si>
-    <t>23.12.2024</t>
   </si>
   <si>
     <t>DA</t>
@@ -973,7 +961,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -984,9 +972,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1072,10 +1057,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1092,9 +1073,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1142,9 +1120,39 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Navadno" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1433,1901 +1441,1903 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BD53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y18" sqref="Y18"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.5" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.5" customWidth="1"/>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" style="4" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" style="4" customWidth="1"/>
-    <col min="12" max="12" width="28.140625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="9.85546875" style="4" customWidth="1"/>
-    <col min="14" max="14" width="32.140625" style="4" customWidth="1"/>
-    <col min="15" max="15" width="22.85546875" style="3" customWidth="1"/>
-    <col min="16" max="16" width="13.85546875" style="3" customWidth="1"/>
-    <col min="17" max="17" width="13.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" style="4" customWidth="1"/>
+    <col min="12" max="12" width="28.1640625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="9.83203125" style="4" customWidth="1"/>
+    <col min="14" max="14" width="32.1640625" style="4" customWidth="1"/>
+    <col min="15" max="15" width="22.83203125" style="3" customWidth="1"/>
+    <col min="16" max="16" width="13.83203125" style="3" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" style="3" customWidth="1"/>
     <col min="18" max="18" width="16" style="3" customWidth="1"/>
-    <col min="19" max="19" width="19.140625" style="3" customWidth="1"/>
+    <col min="19" max="19" width="19.1640625" style="3" customWidth="1"/>
     <col min="20" max="20" width="9" style="3"/>
-    <col min="21" max="21" width="47.140625" style="3" customWidth="1"/>
+    <col min="21" max="21" width="47.1640625" style="3" customWidth="1"/>
     <col min="22" max="22" width="18" style="4" customWidth="1"/>
     <col min="23" max="23" width="12" style="4" customWidth="1"/>
-    <col min="24" max="24" width="13.5703125" style="4" customWidth="1"/>
+    <col min="24" max="24" width="13.5" style="4" customWidth="1"/>
     <col min="25" max="25" width="14" style="4" customWidth="1"/>
-    <col min="26" max="26" width="19.42578125" style="4" customWidth="1"/>
+    <col min="26" max="26" width="19.5" style="4" customWidth="1"/>
     <col min="27" max="27" width="9" style="4"/>
-    <col min="28" max="28" width="25.7109375" style="4" customWidth="1"/>
-    <col min="29" max="29" width="17.5703125" style="3" customWidth="1"/>
+    <col min="28" max="28" width="25.6640625" style="4" customWidth="1"/>
+    <col min="29" max="29" width="17.5" style="3" customWidth="1"/>
     <col min="30" max="30" width="13" style="3" customWidth="1"/>
-    <col min="31" max="31" width="13.42578125" style="3" customWidth="1"/>
-    <col min="32" max="32" width="14.85546875" style="3" customWidth="1"/>
-    <col min="33" max="33" width="14.5703125" style="3" customWidth="1"/>
+    <col min="31" max="31" width="13.5" style="3" customWidth="1"/>
+    <col min="32" max="32" width="14.83203125" style="3" customWidth="1"/>
+    <col min="33" max="33" width="14.5" style="3" customWidth="1"/>
     <col min="34" max="34" width="9" style="3"/>
-    <col min="35" max="35" width="31.5703125" style="3" customWidth="1"/>
-    <col min="36" max="36" width="24.7109375" style="4" customWidth="1"/>
+    <col min="35" max="35" width="31.5" style="3" customWidth="1"/>
+    <col min="36" max="36" width="24.6640625" style="4" customWidth="1"/>
     <col min="37" max="37" width="14" style="4" customWidth="1"/>
-    <col min="38" max="38" width="13.42578125" style="4" customWidth="1"/>
-    <col min="39" max="39" width="14.42578125" style="4" customWidth="1"/>
-    <col min="40" max="40" width="19.85546875" style="4" customWidth="1"/>
+    <col min="38" max="38" width="13.5" style="4" customWidth="1"/>
+    <col min="39" max="39" width="14.5" style="4" customWidth="1"/>
+    <col min="40" max="40" width="19.83203125" style="4" customWidth="1"/>
     <col min="41" max="41" width="9" style="4"/>
-    <col min="42" max="42" width="28.42578125" style="4" customWidth="1"/>
-    <col min="43" max="43" width="18.42578125" style="3" customWidth="1"/>
-    <col min="44" max="44" width="13.28515625" style="3" customWidth="1"/>
-    <col min="45" max="45" width="12.5703125" style="3" customWidth="1"/>
-    <col min="46" max="46" width="15.42578125" style="3" customWidth="1"/>
-    <col min="47" max="47" width="18.7109375" style="3" customWidth="1"/>
+    <col min="42" max="42" width="28.5" style="4" customWidth="1"/>
+    <col min="43" max="43" width="18.5" style="3" customWidth="1"/>
+    <col min="44" max="44" width="13.33203125" style="3" customWidth="1"/>
+    <col min="45" max="45" width="12.5" style="3" customWidth="1"/>
+    <col min="46" max="46" width="15.5" style="3" customWidth="1"/>
+    <col min="47" max="47" width="18.6640625" style="3" customWidth="1"/>
     <col min="48" max="48" width="9" style="3"/>
-    <col min="49" max="49" width="25.42578125" style="3" customWidth="1"/>
-    <col min="50" max="51" width="24.7109375" style="1" customWidth="1"/>
-    <col min="52" max="52" width="19.5703125" customWidth="1"/>
-    <col min="53" max="53" width="29.140625" customWidth="1"/>
-    <col min="54" max="54" width="25.5703125" customWidth="1"/>
+    <col min="49" max="49" width="25.5" style="3" customWidth="1"/>
+    <col min="50" max="51" width="24.6640625" style="1" customWidth="1"/>
+    <col min="52" max="52" width="19.5" customWidth="1"/>
+    <col min="53" max="53" width="29.1640625" customWidth="1"/>
+    <col min="54" max="54" width="25.5" customWidth="1"/>
     <col min="55" max="55" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" ht="48" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="B1" s="35" t="s">
+    <row r="1" spans="1:56" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="11" t="s">
+      <c r="G1" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="P1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="K1" s="11" t="s">
+      <c r="Q1" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="R1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="S1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="T1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="U1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="V1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="W1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="R1" s="12" t="s">
+      <c r="X1" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="Z1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="AA1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="AB1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="V1" s="11" t="s">
+      <c r="AC1" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="W1" s="11" t="s">
+      <c r="AD1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y1" s="11" t="s">
+      <c r="AE1" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="11" t="s">
+      <c r="AG1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="11" t="s">
+      <c r="AH1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="11" t="s">
+      <c r="AI1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="12" t="s">
+      <c r="AJ1" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="AD1" s="12" t="s">
+      <c r="AK1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AE1" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="AF1" s="12" t="s">
+      <c r="AL1" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="AG1" s="12" t="s">
+      <c r="AN1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="AH1" s="12" t="s">
+      <c r="AO1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="AI1" s="12" t="s">
+      <c r="AP1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="AJ1" s="11" t="s">
+      <c r="AQ1" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="AK1" s="11" t="s">
+      <c r="AR1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="AL1" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="AM1" s="11" t="s">
+      <c r="AS1" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AT1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="AN1" s="11" t="s">
+      <c r="AU1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="AO1" s="11" t="s">
+      <c r="AV1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="AP1" s="11" t="s">
+      <c r="AW1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="AQ1" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="AR1" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="AS1" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="AT1" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="AU1" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="AV1" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="AW1" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="AX1" s="36" t="s">
+      <c r="AX1" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="AY1" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="AZ1" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="AY1" s="36" t="s">
-        <v>85</v>
-      </c>
-      <c r="AZ1" s="37" t="s">
+      <c r="BA1" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="BA1" s="36" t="s">
+      <c r="BB1" s="35" t="s">
         <v>57</v>
-      </c>
-      <c r="BB1" s="36" t="s">
-        <v>58</v>
       </c>
       <c r="BC1" s="1"/>
       <c r="BD1" s="1"/>
     </row>
-    <row r="2" spans="1:56" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+    <row r="2" spans="1:56" ht="64" x14ac:dyDescent="0.2">
+      <c r="A2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="36">
+      <c r="B2" s="35">
         <v>24</v>
       </c>
-      <c r="C2" s="36" t="s">
-        <v>95</v>
-      </c>
-      <c r="D2" s="36" t="s">
+      <c r="C2" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="61">
+        <v>45635</v>
+      </c>
+      <c r="G2" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="J2" s="13">
+        <v>24</v>
+      </c>
+      <c r="K2" s="13">
+        <v>1</v>
+      </c>
+      <c r="L2" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="14">
-        <v>24</v>
-      </c>
-      <c r="K2" s="14">
+      <c r="M2" s="13">
+        <v>7</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="12">
+        <v>13</v>
+      </c>
+      <c r="R2" s="12">
         <v>1</v>
       </c>
-      <c r="L2" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="M2" s="14">
+      <c r="S2" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" s="12">
         <v>7</v>
       </c>
-      <c r="N2" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="O2" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="P2" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q2" s="13">
-        <v>13</v>
-      </c>
-      <c r="R2" s="13">
+      <c r="U2" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="V2" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="W2" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="X2" s="13">
+        <v>5</v>
+      </c>
+      <c r="Y2" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="13"/>
+      <c r="AA2" s="13">
+        <v>7</v>
+      </c>
+      <c r="AB2" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC2" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD2" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE2" s="12">
+        <v>7</v>
+      </c>
+      <c r="AF2" s="12">
         <v>1</v>
       </c>
-      <c r="S2" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="T2" s="13">
+      <c r="AG2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="AH2" s="12">
         <v>7</v>
       </c>
-      <c r="U2" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="V2" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="W2" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="X2" s="14">
-        <v>5</v>
-      </c>
-      <c r="Y2" s="14">
+      <c r="AI2" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AJ2" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK2" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL2" s="13">
+        <v>9</v>
+      </c>
+      <c r="AM2" s="13">
         <v>0</v>
       </c>
-      <c r="Z2" s="14"/>
-      <c r="AA2" s="14">
+      <c r="AN2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="AO2" s="13">
         <v>7</v>
       </c>
-      <c r="AB2" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC2" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="AD2" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE2" s="13">
+      <c r="AP2" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="AQ2" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="AR2" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="AS2" s="12">
+        <v>4</v>
+      </c>
+      <c r="AT2" s="12">
+        <v>0</v>
+      </c>
+      <c r="AU2" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="AV2" s="12">
         <v>7</v>
       </c>
-      <c r="AF2" s="13">
-        <v>1</v>
-      </c>
-      <c r="AG2" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="AH2" s="13">
-        <v>7</v>
-      </c>
-      <c r="AI2" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="AJ2" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="AK2" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL2" s="14">
-        <v>9</v>
-      </c>
-      <c r="AM2" s="14">
-        <v>0</v>
-      </c>
-      <c r="AN2" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="AO2" s="14">
-        <v>7</v>
-      </c>
-      <c r="AP2" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ2" s="13" t="s">
+      <c r="AW2" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="AR2" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="AS2" s="13">
-        <v>4</v>
-      </c>
-      <c r="AT2" s="13">
-        <v>0</v>
-      </c>
-      <c r="AU2" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="AV2" s="13">
-        <v>7</v>
-      </c>
-      <c r="AW2" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="AX2" s="36" t="s">
+      <c r="AX2" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="AY2" s="35">
+        <v>8</v>
+      </c>
+      <c r="AZ2" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="AY2" s="36">
-        <v>8</v>
-      </c>
-      <c r="AZ2" s="36" t="s">
+      <c r="BA2" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="BA2" s="36" t="s">
+      <c r="BB2" s="35" t="s">
         <v>61</v>
-      </c>
-      <c r="BB2" s="36" t="s">
-        <v>62</v>
       </c>
       <c r="BC2" s="1"/>
       <c r="BD2" s="1"/>
     </row>
-    <row r="3" spans="1:56" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+    <row r="3" spans="1:56" ht="64" x14ac:dyDescent="0.2">
+      <c r="A3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="36">
+      <c r="B3" s="35">
         <v>23</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="36" t="s">
+      <c r="F3" s="61">
+        <v>45636</v>
+      </c>
+      <c r="G3" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="13">
+        <v>10</v>
+      </c>
+      <c r="K3" s="13">
+        <v>0</v>
+      </c>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13">
+        <v>5.5</v>
+      </c>
+      <c r="N3" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="O3" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" s="12">
+        <v>20</v>
+      </c>
+      <c r="R3" s="12">
+        <v>0</v>
+      </c>
+      <c r="S3" s="12"/>
+      <c r="T3" s="12">
+        <v>4.5</v>
+      </c>
+      <c r="U3" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="14" t="s">
+      <c r="V3" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="W3" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="14">
-        <v>10</v>
-      </c>
-      <c r="K3" s="14">
+      <c r="X3" s="13">
+        <v>13</v>
+      </c>
+      <c r="Y3" s="13">
         <v>0</v>
       </c>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14">
+      <c r="Z3" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA3" s="13">
         <v>5.5</v>
       </c>
-      <c r="N3" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="O3" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="P3" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q3" s="13">
-        <v>20</v>
-      </c>
-      <c r="R3" s="13">
+      <c r="AB3" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC3" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD3" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE3" s="12">
+        <v>18</v>
+      </c>
+      <c r="AF3" s="12">
+        <v>3</v>
+      </c>
+      <c r="AG3" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH3" s="12">
+        <v>4.5</v>
+      </c>
+      <c r="AI3" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ3" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK3" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL3" s="13">
+        <v>15</v>
+      </c>
+      <c r="AM3" s="13"/>
+      <c r="AN3" s="13"/>
+      <c r="AO3" s="13">
+        <v>6</v>
+      </c>
+      <c r="AP3" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="AQ3" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="AR3" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="AS3" s="12">
+        <v>5</v>
+      </c>
+      <c r="AT3" s="12">
         <v>0</v>
       </c>
-      <c r="S3" s="13"/>
-      <c r="T3" s="13">
-        <v>4.5</v>
-      </c>
-      <c r="U3" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="V3" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="W3" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="X3" s="14">
-        <v>13</v>
-      </c>
-      <c r="Y3" s="14">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA3" s="14">
-        <v>5.5</v>
-      </c>
-      <c r="AB3" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC3" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="AD3" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE3" s="13">
-        <v>18</v>
-      </c>
-      <c r="AF3" s="13">
-        <v>3</v>
-      </c>
-      <c r="AG3" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="AH3" s="13">
-        <v>4.5</v>
-      </c>
-      <c r="AI3" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="AJ3" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="AK3" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL3" s="14">
-        <v>15</v>
-      </c>
-      <c r="AM3" s="14"/>
-      <c r="AN3" s="14"/>
-      <c r="AO3" s="14">
-        <v>6</v>
-      </c>
-      <c r="AP3" s="14" t="s">
+      <c r="AU3" s="12"/>
+      <c r="AV3" s="12">
+        <v>5</v>
+      </c>
+      <c r="AW3" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AX3" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="AQ3" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR3" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="AS3" s="13">
-        <v>5</v>
-      </c>
-      <c r="AT3" s="13">
-        <v>0</v>
-      </c>
-      <c r="AU3" s="13"/>
-      <c r="AV3" s="13">
-        <v>5</v>
-      </c>
-      <c r="AW3" s="13" t="s">
+      <c r="AY3" s="37">
+        <v>7</v>
+      </c>
+      <c r="AZ3" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="AX3" s="38" t="s">
+      <c r="BA3" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="AY3" s="38">
-        <v>7</v>
-      </c>
-      <c r="AZ3" s="36" t="s">
+      <c r="BB3" s="35" t="s">
         <v>77</v>
-      </c>
-      <c r="BA3" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="BB3" s="36" t="s">
-        <v>79</v>
       </c>
       <c r="BC3" s="1"/>
       <c r="BD3" s="1"/>
     </row>
-    <row r="4" spans="1:56" ht="240" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
+    <row r="4" spans="1:56" ht="192" x14ac:dyDescent="0.2">
+      <c r="A4" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="36">
+      <c r="B4" s="35">
         <v>23</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="36" t="s">
+      <c r="F4" s="60" t="s">
+        <v>93</v>
+      </c>
+      <c r="G4" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="13">
+        <v>20</v>
+      </c>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13">
+        <v>6</v>
+      </c>
+      <c r="N4" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="P4" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q4" s="12">
+        <v>21</v>
+      </c>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12">
+        <v>4.5</v>
+      </c>
+      <c r="U4" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="V4" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="W4" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="X4" s="13">
+        <v>4</v>
+      </c>
+      <c r="Y4" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="13"/>
+      <c r="AA4" s="13">
+        <v>7</v>
+      </c>
+      <c r="AB4" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="E4" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="F4" s="36" t="s">
-        <v>96</v>
-      </c>
-      <c r="G4" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="14" t="s">
+      <c r="AC4" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD4" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="I4" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="J4" s="14">
-        <v>20</v>
-      </c>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14">
+      <c r="AE4" s="12">
+        <v>5</v>
+      </c>
+      <c r="AF4" s="12"/>
+      <c r="AG4" s="12"/>
+      <c r="AH4" s="12">
+        <v>7</v>
+      </c>
+      <c r="AI4" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="AJ4" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK4" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL4" s="13">
+        <v>10</v>
+      </c>
+      <c r="AM4" s="13"/>
+      <c r="AN4" s="13"/>
+      <c r="AO4" s="13">
         <v>6</v>
       </c>
-      <c r="N4" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="O4" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="P4" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q4" s="13">
-        <v>21</v>
-      </c>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13">
-        <v>4.5</v>
-      </c>
-      <c r="U4" s="13" t="s">
+      <c r="AP4" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="V4" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="W4" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="X4" s="14">
-        <v>4</v>
-      </c>
-      <c r="Y4" s="14">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="14"/>
-      <c r="AA4" s="14">
-        <v>7</v>
-      </c>
-      <c r="AB4" s="14" t="s">
+      <c r="AQ4" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="AR4" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="AS4" s="12">
+        <v>10</v>
+      </c>
+      <c r="AT4" s="12"/>
+      <c r="AU4" s="12"/>
+      <c r="AV4" s="12">
+        <v>6</v>
+      </c>
+      <c r="AW4" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="AC4" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="AD4" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE4" s="13">
-        <v>5</v>
-      </c>
-      <c r="AF4" s="13"/>
-      <c r="AG4" s="13"/>
-      <c r="AH4" s="13">
-        <v>7</v>
-      </c>
-      <c r="AI4" s="13" t="s">
+      <c r="AX4" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="AY4" s="35">
+        <v>10</v>
+      </c>
+      <c r="AZ4" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="AJ4" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="AK4" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL4" s="14">
-        <v>10</v>
-      </c>
-      <c r="AM4" s="14"/>
-      <c r="AN4" s="14"/>
-      <c r="AO4" s="14">
-        <v>6</v>
-      </c>
-      <c r="AP4" s="14" t="s">
+      <c r="BA4" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="AQ4" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR4" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="AS4" s="13">
-        <v>10</v>
-      </c>
-      <c r="AT4" s="13"/>
-      <c r="AU4" s="13"/>
-      <c r="AV4" s="13">
-        <v>6</v>
-      </c>
-      <c r="AW4" s="13" t="s">
+      <c r="BB4" s="38" t="s">
         <v>104</v>
-      </c>
-      <c r="AX4" s="36" t="s">
-        <v>97</v>
-      </c>
-      <c r="AY4" s="36">
-        <v>10</v>
-      </c>
-      <c r="AZ4" s="36" t="s">
-        <v>105</v>
-      </c>
-      <c r="BA4" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="BB4" s="39" t="s">
-        <v>107</v>
       </c>
       <c r="BC4" s="1"/>
       <c r="BD4" s="1"/>
     </row>
-    <row r="5" spans="1:56" ht="120" x14ac:dyDescent="0.25">
-      <c r="A5" s="36" t="s">
+    <row r="5" spans="1:56" ht="96" x14ac:dyDescent="0.2">
+      <c r="A5" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="36">
+      <c r="B5" s="35">
         <v>25</v>
       </c>
-      <c r="C5" s="36" t="s">
-        <v>95</v>
-      </c>
-      <c r="D5" s="36" t="s">
+      <c r="C5" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="61">
+        <v>45637</v>
+      </c>
+      <c r="G5" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="J5" s="13">
+        <v>40</v>
+      </c>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="M5" s="13">
+        <v>3</v>
+      </c>
+      <c r="N5" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="E5" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="40">
-        <v>45649</v>
-      </c>
-      <c r="G5" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" s="14" t="s">
+      <c r="O5" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="P5" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q5" s="12">
+        <v>12</v>
+      </c>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12">
+        <v>0</v>
+      </c>
+      <c r="T5" s="12">
+        <v>7</v>
+      </c>
+      <c r="U5" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="V5" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="W5" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="X5" s="13">
+        <v>10</v>
+      </c>
+      <c r="Y5" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="13">
+        <v>6</v>
+      </c>
+      <c r="AB5" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="J5" s="14">
+      <c r="AC5" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14" t="s">
+      <c r="AD5" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="AE5" s="12">
+        <v>5</v>
+      </c>
+      <c r="AF5" s="12"/>
+      <c r="AG5" s="12">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="12">
+        <v>7</v>
+      </c>
+      <c r="AI5" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="M5" s="14">
+      <c r="AJ5" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK5" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="AL5" s="13">
+        <v>19</v>
+      </c>
+      <c r="AM5" s="13"/>
+      <c r="AN5" s="13">
         <v>3</v>
       </c>
-      <c r="N5" s="14" t="s">
+      <c r="AO5" s="13">
+        <v>5</v>
+      </c>
+      <c r="AP5" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="O5" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="P5" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q5" s="13">
-        <v>12</v>
-      </c>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13">
+      <c r="AQ5" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="AR5" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="AS5" s="12">
+        <v>7</v>
+      </c>
+      <c r="AT5" s="12"/>
+      <c r="AU5" s="12">
+        <v>2</v>
+      </c>
+      <c r="AV5" s="12">
+        <v>6</v>
+      </c>
+      <c r="AW5" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="AX5" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="AY5" s="35">
         <v>0</v>
       </c>
-      <c r="T5" s="13">
-        <v>7</v>
-      </c>
-      <c r="U5" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="V5" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="W5" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="X5" s="14">
-        <v>10</v>
-      </c>
-      <c r="Y5" s="14">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="14">
-        <v>1</v>
-      </c>
-      <c r="AA5" s="14">
-        <v>6</v>
-      </c>
-      <c r="AB5" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="AC5" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="AD5" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="AE5" s="13">
-        <v>5</v>
-      </c>
-      <c r="AF5" s="13"/>
-      <c r="AG5" s="13">
-        <v>0</v>
-      </c>
-      <c r="AH5" s="13">
-        <v>7</v>
-      </c>
-      <c r="AI5" s="13" t="s">
+      <c r="AZ5" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="AJ5" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="AK5" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="AL5" s="14">
-        <v>19</v>
-      </c>
-      <c r="AM5" s="14"/>
-      <c r="AN5" s="14">
-        <v>3</v>
-      </c>
-      <c r="AO5" s="14">
-        <v>5</v>
-      </c>
-      <c r="AP5" s="14" t="s">
+      <c r="BA5" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="AQ5" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR5" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="AS5" s="13">
-        <v>7</v>
-      </c>
-      <c r="AT5" s="13"/>
-      <c r="AU5" s="13">
-        <v>2</v>
-      </c>
-      <c r="AV5" s="13">
-        <v>6</v>
-      </c>
-      <c r="AW5" s="13" t="s">
+      <c r="BB5" s="35" t="s">
         <v>117</v>
-      </c>
-      <c r="AX5" s="36" t="s">
-        <v>118</v>
-      </c>
-      <c r="AY5" s="36">
-        <v>0</v>
-      </c>
-      <c r="AZ5" s="36" t="s">
-        <v>119</v>
-      </c>
-      <c r="BA5" s="35" t="s">
-        <v>120</v>
-      </c>
-      <c r="BB5" s="36" t="s">
-        <v>121</v>
       </c>
       <c r="BC5" s="1"/>
       <c r="BD5" s="1"/>
     </row>
-    <row r="6" spans="1:56" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
+    <row r="6" spans="1:56" ht="80" x14ac:dyDescent="0.2">
+      <c r="A6" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="36">
+      <c r="B6" s="35">
         <v>55</v>
       </c>
-      <c r="C6" s="36" t="s">
-        <v>95</v>
-      </c>
-      <c r="D6" s="36" t="s">
+      <c r="C6" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="E6" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="41">
-        <v>45299</v>
-      </c>
-      <c r="G6" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="I6" s="14" t="s">
+      <c r="F6" s="62">
+        <v>45638</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13">
+        <v>0</v>
+      </c>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13">
+        <v>1</v>
+      </c>
+      <c r="N6" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="O6" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="P6" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q6" s="12">
+        <v>28</v>
+      </c>
+      <c r="R6" s="12">
+        <v>1</v>
+      </c>
+      <c r="S6" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="T6" s="12">
+        <v>7</v>
+      </c>
+      <c r="U6" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="V6" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="W6" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="X6" s="13">
+        <v>13</v>
+      </c>
+      <c r="Y6" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14">
-        <v>0</v>
-      </c>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14">
+      <c r="AA6" s="13">
+        <v>6</v>
+      </c>
+      <c r="AB6" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="AC6" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD6" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="AE6" s="12">
+        <v>28</v>
+      </c>
+      <c r="AF6" s="12"/>
+      <c r="AG6" s="12"/>
+      <c r="AH6" s="12">
+        <v>5</v>
+      </c>
+      <c r="AI6" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="AJ6" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK6" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="AL6" s="13">
+        <v>13</v>
+      </c>
+      <c r="AM6" s="13"/>
+      <c r="AN6" s="13"/>
+      <c r="AO6" s="13">
+        <v>7</v>
+      </c>
+      <c r="AP6" s="13"/>
+      <c r="AQ6" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="AR6" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="AS6" s="12">
+        <v>13</v>
+      </c>
+      <c r="AT6" s="12">
         <v>1</v>
       </c>
-      <c r="N6" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="O6" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="P6" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q6" s="13">
-        <v>28</v>
-      </c>
-      <c r="R6" s="13">
-        <v>1</v>
-      </c>
-      <c r="S6" s="13" t="s">
+      <c r="AU6" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="T6" s="13">
-        <v>7</v>
-      </c>
-      <c r="U6" s="13" t="s">
+      <c r="AV6" s="12">
+        <v>6</v>
+      </c>
+      <c r="AW6" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="V6" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="W6" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="X6" s="14">
-        <v>13</v>
-      </c>
-      <c r="Y6" s="14">
-        <v>1</v>
-      </c>
-      <c r="Z6" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="AA6" s="14">
-        <v>6</v>
-      </c>
-      <c r="AB6" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="AC6" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="AD6" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="AE6" s="13">
-        <v>28</v>
-      </c>
-      <c r="AF6" s="13"/>
-      <c r="AG6" s="13"/>
-      <c r="AH6" s="13">
-        <v>5</v>
-      </c>
-      <c r="AI6" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="AJ6" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="AK6" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="AL6" s="14">
-        <v>13</v>
-      </c>
-      <c r="AM6" s="14"/>
-      <c r="AN6" s="14"/>
-      <c r="AO6" s="14">
-        <v>7</v>
-      </c>
-      <c r="AP6" s="14"/>
-      <c r="AQ6" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR6" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="AS6" s="13">
-        <v>13</v>
-      </c>
-      <c r="AT6" s="13">
-        <v>1</v>
-      </c>
-      <c r="AU6" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="AV6" s="13">
-        <v>6</v>
-      </c>
-      <c r="AW6" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="AX6" s="36"/>
-      <c r="AY6" s="36">
+      <c r="AX6" s="35"/>
+      <c r="AY6" s="35">
         <v>8</v>
       </c>
-      <c r="AZ6" s="36" t="s">
-        <v>173</v>
-      </c>
-      <c r="BA6" s="38" t="s">
-        <v>174</v>
-      </c>
-      <c r="BB6" s="36" t="s">
-        <v>175</v>
+      <c r="AZ6" s="35" t="s">
+        <v>169</v>
+      </c>
+      <c r="BA6" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="BB6" s="35" t="s">
+        <v>171</v>
       </c>
       <c r="BC6" s="1"/>
       <c r="BD6" s="1"/>
     </row>
-    <row r="7" spans="1:56" ht="120" x14ac:dyDescent="0.25">
-      <c r="A7" s="42" t="s">
+    <row r="7" spans="1:56" ht="112" x14ac:dyDescent="0.2">
+      <c r="A7" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="43">
+      <c r="B7" s="40">
         <v>53</v>
       </c>
-      <c r="C7" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="D7" s="34" t="s">
+      <c r="C7" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="63">
+        <v>45639</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="42" t="s">
+        <v>131</v>
+      </c>
+      <c r="J7" s="42"/>
+      <c r="K7" s="42">
+        <v>1</v>
+      </c>
+      <c r="L7" s="42" t="s">
+        <v>140</v>
+      </c>
+      <c r="M7" s="42">
+        <v>1</v>
+      </c>
+      <c r="N7" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="O7" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="P7" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q7" s="43"/>
+      <c r="R7" s="43">
+        <v>1</v>
+      </c>
+      <c r="S7" s="43" t="s">
+        <v>142</v>
+      </c>
+      <c r="T7" s="43">
+        <v>1</v>
+      </c>
+      <c r="U7" s="43" t="s">
         <v>143</v>
       </c>
-      <c r="E7" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="34"/>
-      <c r="G7" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="I7" s="45" t="s">
-        <v>135</v>
-      </c>
-      <c r="J7" s="45"/>
-      <c r="K7" s="45">
+      <c r="V7" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="W7" s="42" t="s">
+        <v>131</v>
+      </c>
+      <c r="X7" s="42"/>
+      <c r="Y7" s="42">
         <v>1</v>
       </c>
-      <c r="L7" s="45" t="s">
+      <c r="Z7" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="M7" s="45">
+      <c r="AA7" s="42">
+        <v>5</v>
+      </c>
+      <c r="AB7" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="AC7" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD7" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="AE7" s="43"/>
+      <c r="AF7" s="43">
         <v>1</v>
       </c>
-      <c r="N7" s="45" t="s">
-        <v>145</v>
-      </c>
-      <c r="O7" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="P7" s="46" t="s">
-        <v>135</v>
-      </c>
-      <c r="Q7" s="46"/>
-      <c r="R7" s="46">
+      <c r="AG7" s="43" t="s">
+        <v>146</v>
+      </c>
+      <c r="AH7" s="43">
         <v>1</v>
       </c>
-      <c r="S7" s="46" t="s">
-        <v>146</v>
-      </c>
-      <c r="T7" s="46">
+      <c r="AI7" s="43" t="s">
+        <v>147</v>
+      </c>
+      <c r="AJ7" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK7" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="AL7" s="42">
+        <v>55</v>
+      </c>
+      <c r="AM7" s="42">
         <v>1</v>
       </c>
-      <c r="U7" s="46" t="s">
-        <v>147</v>
-      </c>
-      <c r="V7" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="W7" s="45" t="s">
-        <v>135</v>
-      </c>
-      <c r="X7" s="45"/>
-      <c r="Y7" s="45">
+      <c r="AN7" s="42" t="s">
+        <v>148</v>
+      </c>
+      <c r="AO7" s="42">
+        <v>3</v>
+      </c>
+      <c r="AP7" s="42" t="s">
+        <v>149</v>
+      </c>
+      <c r="AQ7" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="AR7" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="AS7" s="43">
+        <v>24</v>
+      </c>
+      <c r="AT7" s="43">
         <v>1</v>
       </c>
-      <c r="Z7" s="45" t="s">
-        <v>148</v>
-      </c>
-      <c r="AA7" s="45">
-        <v>5</v>
-      </c>
-      <c r="AB7" s="45" t="s">
-        <v>149</v>
-      </c>
-      <c r="AC7" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="AD7" s="46" t="s">
-        <v>135</v>
-      </c>
-      <c r="AE7" s="46"/>
-      <c r="AF7" s="46">
-        <v>1</v>
-      </c>
-      <c r="AG7" s="46" t="s">
+      <c r="AU7" s="43" t="s">
         <v>150</v>
       </c>
-      <c r="AH7" s="46">
-        <v>1</v>
-      </c>
-      <c r="AI7" s="46" t="s">
+      <c r="AV7" s="43">
+        <v>4</v>
+      </c>
+      <c r="AW7" s="44" t="s">
         <v>151</v>
       </c>
-      <c r="AJ7" s="45" t="s">
-        <v>50</v>
-      </c>
-      <c r="AK7" s="45" t="s">
-        <v>110</v>
-      </c>
-      <c r="AL7" s="45">
-        <v>55</v>
-      </c>
-      <c r="AM7" s="45">
-        <v>1</v>
-      </c>
-      <c r="AN7" s="45" t="s">
-        <v>152</v>
-      </c>
-      <c r="AO7" s="45">
+      <c r="AX7" s="40"/>
+      <c r="AY7" s="33">
         <v>3</v>
       </c>
-      <c r="AP7" s="45" t="s">
-        <v>153</v>
-      </c>
-      <c r="AQ7" s="46" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR7" s="46" t="s">
-        <v>110</v>
-      </c>
-      <c r="AS7" s="46">
-        <v>24</v>
-      </c>
-      <c r="AT7" s="46">
-        <v>1</v>
-      </c>
-      <c r="AU7" s="46" t="s">
-        <v>154</v>
-      </c>
-      <c r="AV7" s="46">
-        <v>4</v>
-      </c>
-      <c r="AW7" s="47" t="s">
-        <v>155</v>
-      </c>
-      <c r="AX7" s="43"/>
-      <c r="AY7" s="34">
-        <v>3</v>
-      </c>
-      <c r="AZ7" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="BA7" s="34" t="s">
-        <v>177</v>
-      </c>
-      <c r="BB7" s="22" t="s">
-        <v>178</v>
+      <c r="AZ7" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="BA7" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="BB7" s="21" t="s">
+        <v>174</v>
       </c>
       <c r="BC7" s="1"/>
       <c r="BD7" s="1"/>
     </row>
-    <row r="8" spans="1:56" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
-        <v>168</v>
-      </c>
-      <c r="B8" s="34">
+    <row r="8" spans="1:56" ht="96" x14ac:dyDescent="0.2">
+      <c r="A8" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="B8" s="33">
         <v>49</v>
       </c>
-      <c r="C8" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="D8" s="34" t="s">
-        <v>135</v>
-      </c>
-      <c r="E8" s="34" t="s">
+      <c r="C8" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="F8" s="63">
+        <v>45639</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="J8" s="13">
+        <v>20</v>
+      </c>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13">
+        <v>7</v>
+      </c>
+      <c r="N8" s="13"/>
+      <c r="O8" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="P8" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q8" s="12">
+        <v>22</v>
+      </c>
+      <c r="R8" s="12"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="12">
+        <v>7</v>
+      </c>
+      <c r="U8" s="12"/>
+      <c r="V8" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="W8" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="X8" s="13">
+        <v>60</v>
+      </c>
+      <c r="Y8" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="F8" s="48">
-        <v>45665</v>
-      </c>
-      <c r="G8" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="J8" s="14">
+      <c r="AA8" s="13">
+        <v>1</v>
+      </c>
+      <c r="AB8" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="AC8" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD8" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="AE8" s="12">
+        <v>43</v>
+      </c>
+      <c r="AF8" s="12">
+        <v>1</v>
+      </c>
+      <c r="AG8" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH8" s="12">
+        <v>7</v>
+      </c>
+      <c r="AI8" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="AJ8" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK8" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="AL8" s="13">
+        <v>240</v>
+      </c>
+      <c r="AM8" s="13">
+        <v>1</v>
+      </c>
+      <c r="AN8" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="AO8" s="13">
+        <v>2</v>
+      </c>
+      <c r="AP8" s="13"/>
+      <c r="AQ8" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="AR8" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="AS8" s="12">
         <v>20</v>
       </c>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14">
-        <v>7</v>
-      </c>
-      <c r="N8" s="14"/>
-      <c r="O8" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="P8" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q8" s="13">
-        <v>22</v>
-      </c>
-      <c r="R8" s="13"/>
-      <c r="S8" s="13"/>
-      <c r="T8" s="13">
-        <v>7</v>
-      </c>
-      <c r="U8" s="13"/>
-      <c r="V8" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="W8" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="X8" s="14">
-        <v>60</v>
-      </c>
-      <c r="Y8" s="14">
+      <c r="AT8" s="12">
         <v>1</v>
       </c>
-      <c r="Z8" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="AA8" s="14">
-        <v>1</v>
-      </c>
-      <c r="AB8" s="14" t="s">
+      <c r="AU8" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="AC8" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="AD8" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="AE8" s="13">
-        <v>43</v>
-      </c>
-      <c r="AF8" s="13">
-        <v>1</v>
-      </c>
-      <c r="AG8" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="AH8" s="13">
-        <v>7</v>
-      </c>
-      <c r="AI8" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="AJ8" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="AK8" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="AL8" s="14">
-        <v>240</v>
-      </c>
-      <c r="AM8" s="14">
-        <v>1</v>
-      </c>
-      <c r="AN8" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="AO8" s="14">
-        <v>2</v>
-      </c>
-      <c r="AP8" s="14"/>
-      <c r="AQ8" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR8" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="AS8" s="13">
-        <v>20</v>
-      </c>
-      <c r="AT8" s="13">
-        <v>1</v>
-      </c>
-      <c r="AU8" s="13" t="s">
+      <c r="AV8" s="12">
+        <v>4</v>
+      </c>
+      <c r="AW8" s="20"/>
+      <c r="AX8" s="40"/>
+      <c r="AY8" s="33">
+        <v>5</v>
+      </c>
+      <c r="AZ8" s="33" t="s">
         <v>165</v>
       </c>
-      <c r="AV8" s="13">
-        <v>4</v>
-      </c>
-      <c r="AW8" s="21"/>
-      <c r="AX8" s="43"/>
-      <c r="AY8" s="34">
-        <v>5</v>
-      </c>
-      <c r="AZ8" s="34" t="s">
-        <v>169</v>
-      </c>
-      <c r="BA8" s="34"/>
-      <c r="BB8" s="22" t="s">
-        <v>170</v>
+      <c r="BA8" s="33"/>
+      <c r="BB8" s="21" t="s">
+        <v>166</v>
       </c>
       <c r="BC8" s="1"/>
       <c r="BD8" s="1"/>
     </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="9"/>
-      <c r="T9" s="9"/>
-      <c r="U9" s="9"/>
-      <c r="V9" s="9"/>
-      <c r="W9" s="9"/>
-      <c r="X9" s="9"/>
-      <c r="Y9" s="9"/>
-      <c r="Z9" s="9"/>
-      <c r="AA9" s="9"/>
-      <c r="AB9" s="9"/>
-      <c r="AC9" s="9"/>
-      <c r="AD9" s="9"/>
-      <c r="AE9" s="9"/>
-      <c r="AF9" s="9"/>
-      <c r="AG9" s="9"/>
-      <c r="AH9" s="9"/>
-      <c r="AI9" s="9"/>
-      <c r="AJ9" s="9"/>
-      <c r="AK9" s="9"/>
-      <c r="AL9" s="9"/>
-      <c r="AM9" s="9"/>
-      <c r="AN9" s="9"/>
-      <c r="AO9" s="9"/>
-      <c r="AP9" s="9"/>
-      <c r="AQ9" s="9"/>
-      <c r="AR9" s="9"/>
-      <c r="AS9" s="9"/>
-      <c r="AT9" s="9"/>
-      <c r="AU9" s="9"/>
-      <c r="AV9" s="9"/>
-      <c r="AW9" s="9"/>
-      <c r="AX9" s="9"/>
-      <c r="AY9" s="9"/>
-      <c r="AZ9" s="9"/>
-      <c r="BA9" s="9"/>
-      <c r="BB9" s="9"/>
+    <row r="9" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="8"/>
+      <c r="Y9" s="8"/>
+      <c r="Z9" s="8"/>
+      <c r="AA9" s="8"/>
+      <c r="AB9" s="8"/>
+      <c r="AC9" s="8"/>
+      <c r="AD9" s="8"/>
+      <c r="AE9" s="8"/>
+      <c r="AF9" s="8"/>
+      <c r="AG9" s="8"/>
+      <c r="AH9" s="8"/>
+      <c r="AI9" s="8"/>
+      <c r="AJ9" s="8"/>
+      <c r="AK9" s="8"/>
+      <c r="AL9" s="8"/>
+      <c r="AM9" s="8"/>
+      <c r="AN9" s="8"/>
+      <c r="AO9" s="8"/>
+      <c r="AP9" s="8"/>
+      <c r="AQ9" s="8"/>
+      <c r="AR9" s="8"/>
+      <c r="AS9" s="8"/>
+      <c r="AT9" s="8"/>
+      <c r="AU9" s="8"/>
+      <c r="AV9" s="8"/>
+      <c r="AW9" s="8"/>
+      <c r="AX9" s="8"/>
+      <c r="AY9" s="8"/>
+      <c r="AZ9" s="8"/>
+      <c r="BA9" s="8"/>
+      <c r="BB9" s="8"/>
       <c r="BC9" s="1"/>
       <c r="BD9" s="1"/>
     </row>
-    <row r="10" spans="1:56" ht="21" x14ac:dyDescent="0.35">
-      <c r="A10" s="19"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
-      <c r="U10" s="9"/>
-      <c r="V10" s="9"/>
-      <c r="W10" s="9"/>
-      <c r="X10" s="9"/>
-      <c r="Y10" s="9"/>
-      <c r="Z10" s="9"/>
-      <c r="AA10" s="9"/>
-      <c r="AB10" s="9"/>
-      <c r="AC10" s="9"/>
-      <c r="AD10" s="9"/>
-      <c r="AE10" s="9"/>
-      <c r="AF10" s="9"/>
-      <c r="AG10" s="9"/>
-      <c r="AH10" s="9"/>
-      <c r="AI10" s="9"/>
-      <c r="AJ10" s="9"/>
-      <c r="AK10" s="9"/>
-      <c r="AL10" s="9"/>
-      <c r="AM10" s="9"/>
-      <c r="AN10" s="9"/>
-      <c r="AO10" s="9"/>
-      <c r="AP10" s="9"/>
-      <c r="AQ10" s="9"/>
-      <c r="AR10" s="9"/>
-      <c r="AS10" s="9"/>
-      <c r="AT10" s="9"/>
-      <c r="AU10" s="9"/>
-      <c r="AV10" s="9"/>
-      <c r="AW10" s="9"/>
-      <c r="AX10" s="9"/>
-      <c r="AY10" s="9"/>
-      <c r="AZ10" s="9"/>
-      <c r="BA10" s="9"/>
-      <c r="BB10" s="9"/>
+    <row r="10" spans="1:56" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="8"/>
+      <c r="Y10" s="8"/>
+      <c r="Z10" s="8"/>
+      <c r="AA10" s="8"/>
+      <c r="AB10" s="8"/>
+      <c r="AC10" s="8"/>
+      <c r="AD10" s="8"/>
+      <c r="AE10" s="8"/>
+      <c r="AF10" s="8"/>
+      <c r="AG10" s="8"/>
+      <c r="AH10" s="8"/>
+      <c r="AI10" s="8"/>
+      <c r="AJ10" s="8"/>
+      <c r="AK10" s="8"/>
+      <c r="AL10" s="8"/>
+      <c r="AM10" s="8"/>
+      <c r="AN10" s="8"/>
+      <c r="AO10" s="8"/>
+      <c r="AP10" s="8"/>
+      <c r="AQ10" s="8"/>
+      <c r="AR10" s="8"/>
+      <c r="AS10" s="8"/>
+      <c r="AT10" s="8"/>
+      <c r="AU10" s="8"/>
+      <c r="AV10" s="8"/>
+      <c r="AW10" s="8"/>
+      <c r="AX10" s="8"/>
+      <c r="AY10" s="8"/>
+      <c r="AZ10" s="8"/>
+      <c r="BA10" s="8"/>
+      <c r="BB10" s="8"/>
       <c r="BC10" s="1"/>
       <c r="BD10" s="1"/>
     </row>
-    <row r="11" spans="1:56" ht="61.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="B11" s="29" t="s">
+    <row r="11" spans="1:56" ht="49" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="B11" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="30" t="s">
+      <c r="F11" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="11" t="s">
+      <c r="G11" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M11" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="N11" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="O11" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="P11" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="J11" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="K11" s="11" t="s">
+      <c r="Q11" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="R11" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="L11" s="11" t="s">
+      <c r="S11" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="M11" s="11" t="s">
+      <c r="T11" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="N11" s="11" t="s">
+      <c r="U11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="O11" s="12" t="s">
+      <c r="V11" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="P11" s="12" t="s">
+      <c r="W11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="Q11" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="R11" s="12" t="s">
+      <c r="X11" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y11" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="S11" s="12" t="s">
+      <c r="Z11" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="T11" s="12" t="s">
+      <c r="AA11" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="U11" s="12" t="s">
+      <c r="AB11" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="V11" s="11" t="s">
+      <c r="AC11" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="W11" s="11" t="s">
+      <c r="AD11" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="X11" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y11" s="11" t="s">
+      <c r="AE11" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF11" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="Z11" s="11" t="s">
+      <c r="AG11" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="AA11" s="11" t="s">
+      <c r="AH11" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="AB11" s="11" t="s">
+      <c r="AI11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="AC11" s="12" t="s">
+      <c r="AJ11" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="AD11" s="12" t="s">
+      <c r="AK11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AE11" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="AF11" s="12" t="s">
+      <c r="AL11" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM11" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="AG11" s="12" t="s">
+      <c r="AN11" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="AH11" s="12" t="s">
+      <c r="AO11" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="AI11" s="12" t="s">
+      <c r="AP11" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="AJ11" s="11" t="s">
+      <c r="AQ11" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="AK11" s="11" t="s">
+      <c r="AR11" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="AL11" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="AM11" s="11" t="s">
+      <c r="AS11" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AT11" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="AN11" s="11" t="s">
+      <c r="AU11" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="AO11" s="11" t="s">
+      <c r="AV11" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="AP11" s="11" t="s">
+      <c r="AW11" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="AQ11" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="AR11" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="AS11" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="AT11" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="AU11" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="AV11" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="AW11" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="AX11" s="23" t="s">
+      <c r="AX11" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AY11" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="AZ11" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="AY11" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="AZ11" s="28" t="s">
+      <c r="BA11" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="BA11" s="23" t="s">
+      <c r="BB11" s="26" t="s">
         <v>57</v>
-      </c>
-      <c r="BB11" s="27" t="s">
-        <v>58</v>
       </c>
       <c r="BC11" s="1"/>
       <c r="BD11" s="1"/>
     </row>
-    <row r="12" spans="1:56" ht="135" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
+    <row r="12" spans="1:56" ht="112" x14ac:dyDescent="0.2">
+      <c r="A12" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="21">
         <v>23</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="F12" s="69">
+        <v>45636</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="J12" s="13">
+        <v>30</v>
+      </c>
+      <c r="K12" s="13">
+        <v>0</v>
+      </c>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13">
+        <v>5</v>
+      </c>
+      <c r="N12" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="O12" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="P12" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q12" s="12">
+        <v>120</v>
+      </c>
+      <c r="R12" s="12"/>
+      <c r="S12" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="T12" s="12">
+        <v>5</v>
+      </c>
+      <c r="U12" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="V12" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="W12" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="X12" s="13">
+        <v>20</v>
+      </c>
+      <c r="Y12" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z12" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="E12" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" s="23" t="s">
+      <c r="AA12" s="13">
+        <v>7</v>
+      </c>
+      <c r="AB12" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC12" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD12" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE12" s="12">
+        <v>8</v>
+      </c>
+      <c r="AF12" s="12"/>
+      <c r="AG12" s="12"/>
+      <c r="AH12" s="12">
+        <v>7</v>
+      </c>
+      <c r="AI12" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="AJ12" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK12" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL12" s="13">
+        <v>5</v>
+      </c>
+      <c r="AM12" s="13"/>
+      <c r="AN12" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="AO12" s="13">
+        <v>7</v>
+      </c>
+      <c r="AP12" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="AQ12" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="AR12" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="AS12" s="12">
+        <v>15</v>
+      </c>
+      <c r="AT12" s="12">
+        <v>2</v>
+      </c>
+      <c r="AU12" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="G12" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="H12" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="J12" s="14">
-        <v>30</v>
-      </c>
-      <c r="K12" s="14">
-        <v>0</v>
-      </c>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14">
-        <v>5</v>
-      </c>
-      <c r="N12" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="O12" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="P12" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q12" s="13">
-        <v>120</v>
-      </c>
-      <c r="R12" s="13"/>
-      <c r="S12" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="T12" s="13">
-        <v>5</v>
-      </c>
-      <c r="U12" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="V12" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="W12" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="X12" s="14">
-        <v>20</v>
-      </c>
-      <c r="Y12" s="14">
-        <v>1</v>
-      </c>
-      <c r="Z12" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="AA12" s="14">
-        <v>7</v>
-      </c>
-      <c r="AB12" s="14" t="s">
+      <c r="AV12" s="12">
+        <v>6</v>
+      </c>
+      <c r="AW12" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="AC12" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="AD12" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE12" s="13">
-        <v>8</v>
-      </c>
-      <c r="AF12" s="13"/>
-      <c r="AG12" s="13"/>
-      <c r="AH12" s="13">
-        <v>7</v>
-      </c>
-      <c r="AI12" s="13" t="s">
+      <c r="AX12" s="22"/>
+      <c r="AY12" s="22">
+        <v>6</v>
+      </c>
+      <c r="AZ12" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="AJ12" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="AK12" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL12" s="14">
-        <v>5</v>
-      </c>
-      <c r="AM12" s="14"/>
-      <c r="AN12" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="AO12" s="14">
-        <v>7</v>
-      </c>
-      <c r="AP12" s="14" t="s">
+      <c r="BA12" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="AQ12" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR12" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="AS12" s="13">
-        <v>15</v>
-      </c>
-      <c r="AT12" s="13">
-        <v>2</v>
-      </c>
-      <c r="AU12" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="AV12" s="13">
-        <v>6</v>
-      </c>
-      <c r="AW12" s="21" t="s">
+      <c r="BB12" s="21" t="s">
         <v>91</v>
-      </c>
-      <c r="AX12" s="23"/>
-      <c r="AY12" s="23">
-        <v>6</v>
-      </c>
-      <c r="AZ12" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="BA12" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="BB12" s="22" t="s">
-        <v>94</v>
       </c>
       <c r="BC12" s="1"/>
       <c r="BD12" s="1"/>
     </row>
-    <row r="13" spans="1:56" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:56" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="14">
         <v>27</v>
       </c>
-      <c r="C13" s="16" t="s">
-        <v>95</v>
+      <c r="C13" s="15" t="s">
+        <v>92</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>109</v>
+        <v>63</v>
+      </c>
+      <c r="F13" s="68">
+        <v>45639</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="H13" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="J13" s="6">
+        <v>16</v>
+      </c>
+      <c r="K13" s="6">
+        <v>1</v>
+      </c>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6">
+        <v>6</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="O13" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="P13" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q13" s="7">
         <v>32</v>
       </c>
-      <c r="I13" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="J13" s="7">
-        <v>16</v>
-      </c>
-      <c r="K13" s="7">
+      <c r="R13" s="7">
+        <v>3</v>
+      </c>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7">
+        <v>5</v>
+      </c>
+      <c r="U13" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="V13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="W13" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="X13" s="6">
+        <v>17</v>
+      </c>
+      <c r="Y13" s="6">
         <v>1</v>
       </c>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7">
+      <c r="Z13" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA13" s="6">
+        <v>3</v>
+      </c>
+      <c r="AB13" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="AC13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD13" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="AE13" s="7">
+        <v>9</v>
+      </c>
+      <c r="AF13" s="7">
+        <v>1</v>
+      </c>
+      <c r="AG13" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="AH13" s="7">
         <v>6</v>
       </c>
-      <c r="N13" s="7" t="s">
+      <c r="AI13" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="O13" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="P13" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q13" s="8">
-        <v>32</v>
-      </c>
-      <c r="R13" s="8">
-        <v>3</v>
-      </c>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8">
+      <c r="AJ13" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK13" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="AL13" s="6">
+        <v>7</v>
+      </c>
+      <c r="AM13" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN13" s="6"/>
+      <c r="AO13" s="6">
+        <v>7</v>
+      </c>
+      <c r="AP13" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="AQ13" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="AR13" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="AS13" s="7">
+        <v>12</v>
+      </c>
+      <c r="AT13" s="7">
+        <v>1</v>
+      </c>
+      <c r="AU13" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AV13" s="7">
         <v>5</v>
       </c>
-      <c r="U13" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="V13" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="W13" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="X13" s="7">
-        <v>17</v>
-      </c>
-      <c r="Y13" s="7">
-        <v>1</v>
-      </c>
-      <c r="Z13" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="AA13" s="7">
-        <v>3</v>
-      </c>
-      <c r="AB13" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="AC13" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AD13" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="AE13" s="8">
-        <v>9</v>
-      </c>
-      <c r="AF13" s="8">
-        <v>1</v>
-      </c>
-      <c r="AG13" s="8" t="s">
+      <c r="AW13" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="AX13" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="AH13" s="8">
-        <v>6</v>
-      </c>
-      <c r="AI13" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="AJ13" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="AK13" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="AL13" s="7">
-        <v>7</v>
-      </c>
-      <c r="AM13" s="7">
-        <v>0</v>
-      </c>
-      <c r="AN13" s="7"/>
-      <c r="AO13" s="7">
-        <v>7</v>
-      </c>
-      <c r="AP13" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="AQ13" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR13" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="AS13" s="8">
-        <v>12</v>
-      </c>
-      <c r="AT13" s="8">
-        <v>1</v>
-      </c>
-      <c r="AU13" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="AV13" s="8">
-        <v>5</v>
-      </c>
-      <c r="AW13" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="AX13" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="AY13" s="1">
         <v>0</v>
       </c>
       <c r="AZ13" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="BA13" s="26" t="s">
-        <v>133</v>
+        <v>128</v>
+      </c>
+      <c r="BA13" s="25" t="s">
+        <v>129</v>
       </c>
       <c r="BB13" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="BC13" s="1"/>
       <c r="BD13" s="1"/>
     </row>
-    <row r="14" spans="1:56" ht="105" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:56" ht="96" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
@@ -3335,25 +3345,25 @@
         <v>27</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F14" s="6">
-        <v>45664</v>
+        <v>152</v>
+      </c>
+      <c r="F14" s="68">
+        <v>45640</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="J14" s="5">
         <v>13</v>
@@ -3362,19 +3372,19 @@
         <v>1</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="M14" s="5">
         <v>6</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="Q14" s="2">
         <v>120</v>
@@ -3383,17 +3393,17 @@
         <v>1</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="T14" s="2">
         <v>4</v>
       </c>
       <c r="U14" s="2"/>
       <c r="V14" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="W14" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="X14" s="5">
         <v>5</v>
@@ -3407,10 +3417,10 @@
       </c>
       <c r="AB14" s="5"/>
       <c r="AC14" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AD14" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="AE14" s="2">
         <v>5</v>
@@ -3422,10 +3432,10 @@
       </c>
       <c r="AI14" s="2"/>
       <c r="AJ14" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AK14" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="AL14" s="5">
         <v>4</v>
@@ -3437,10 +3447,10 @@
       </c>
       <c r="AP14" s="5"/>
       <c r="AQ14" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AR14" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="AS14" s="2">
         <v>30</v>
@@ -3453,22 +3463,22 @@
         <v>6</v>
       </c>
       <c r="AW14" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="AY14" s="1">
         <v>6</v>
       </c>
       <c r="AZ14" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="BA14" s="1"/>
       <c r="BB14" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="BC14" s="1"/>
       <c r="BD14" s="1"/>
     </row>
-    <row r="15" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:56" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
@@ -3476,7 +3486,7 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="6"/>
+      <c r="F15" s="68"/>
       <c r="G15" s="1"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
@@ -3526,7 +3536,7 @@
       <c r="BC15" s="1"/>
       <c r="BD15" s="1"/>
     </row>
-    <row r="16" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:56" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
@@ -3534,7 +3544,7 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="F16" s="67"/>
       <c r="G16" s="1"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
@@ -3584,7 +3594,7 @@
       <c r="BC16" s="1"/>
       <c r="BD16" s="1"/>
     </row>
-    <row r="17" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:56" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
@@ -3592,7 +3602,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="F17" s="67"/>
       <c r="G17" s="1"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
@@ -3642,7 +3652,7 @@
       <c r="BC17" s="1"/>
       <c r="BD17" s="1"/>
     </row>
-    <row r="18" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:56" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
@@ -3650,7 +3660,7 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="F18" s="67"/>
       <c r="G18" s="1"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
@@ -3700,7 +3710,7 @@
       <c r="BC18" s="1"/>
       <c r="BD18" s="1"/>
     </row>
-    <row r="19" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:56" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
@@ -3752,15 +3762,15 @@
       <c r="AU19" s="2"/>
       <c r="AV19" s="2"/>
       <c r="AW19" s="2"/>
-      <c r="AX19" s="51"/>
-      <c r="AY19" s="36"/>
-      <c r="AZ19" s="36"/>
-      <c r="BA19" s="36"/>
-      <c r="BB19" s="52"/>
+      <c r="AX19" s="47"/>
+      <c r="AY19" s="35"/>
+      <c r="AZ19" s="35"/>
+      <c r="BA19" s="35"/>
+      <c r="BB19" s="48"/>
       <c r="BC19" s="1"/>
       <c r="BD19" s="1"/>
     </row>
-    <row r="20" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:56" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
@@ -3812,174 +3822,174 @@
       <c r="AU20" s="2"/>
       <c r="AV20" s="2"/>
       <c r="AW20" s="2"/>
-      <c r="AX20" s="53"/>
-      <c r="AY20" s="43"/>
-      <c r="AZ20" s="27"/>
-      <c r="BA20" s="36"/>
-      <c r="BB20" s="54"/>
+      <c r="AX20" s="49"/>
+      <c r="AY20" s="40"/>
+      <c r="AZ20" s="26"/>
+      <c r="BA20" s="35"/>
+      <c r="BB20" s="50"/>
       <c r="BC20" s="1"/>
       <c r="BD20" s="1"/>
     </row>
-    <row r="21" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:56" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B21" s="1">
         <f>AVERAGE(B2:B10)</f>
         <v>36</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-      <c r="H21" s="50"/>
-      <c r="I21" s="50" t="s">
-        <v>188</v>
-      </c>
-      <c r="J21" s="50">
+      <c r="H21" s="46"/>
+      <c r="I21" s="46" t="s">
+        <v>184</v>
+      </c>
+      <c r="J21" s="46">
         <f t="shared" ref="J21:AY21" si="0">AVERAGE(J2:J10)</f>
         <v>22.8</v>
       </c>
-      <c r="K21" s="50">
+      <c r="K21" s="46">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="L21" s="50"/>
-      <c r="M21" s="50">
+      <c r="L21" s="46"/>
+      <c r="M21" s="46">
         <f t="shared" si="0"/>
         <v>4.3571428571428568</v>
       </c>
-      <c r="N21" s="50"/>
-      <c r="O21" s="49"/>
-      <c r="P21" s="49" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q21" s="49">
+      <c r="N21" s="46"/>
+      <c r="O21" s="45"/>
+      <c r="P21" s="45" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q21" s="45">
         <f t="shared" si="0"/>
         <v>19.333333333333332</v>
       </c>
-      <c r="R21" s="49">
+      <c r="R21" s="45">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="S21" s="49"/>
-      <c r="T21" s="49">
+      <c r="S21" s="45"/>
+      <c r="T21" s="45">
         <f t="shared" si="0"/>
         <v>5.4285714285714288</v>
       </c>
-      <c r="U21" s="49"/>
-      <c r="V21" s="50"/>
-      <c r="W21" s="50" t="s">
-        <v>188</v>
-      </c>
-      <c r="X21" s="50">
+      <c r="U21" s="45"/>
+      <c r="V21" s="46"/>
+      <c r="W21" s="46" t="s">
+        <v>184</v>
+      </c>
+      <c r="X21" s="46">
         <f t="shared" si="0"/>
         <v>17.5</v>
       </c>
-      <c r="Y21" s="50">
+      <c r="Y21" s="46">
         <f t="shared" si="0"/>
         <v>0.42857142857142855</v>
       </c>
-      <c r="Z21" s="50"/>
-      <c r="AA21" s="50">
+      <c r="Z21" s="46"/>
+      <c r="AA21" s="46">
         <f t="shared" si="0"/>
         <v>5.3571428571428568</v>
       </c>
-      <c r="AB21" s="50"/>
-      <c r="AC21" s="49"/>
-      <c r="AD21" s="49" t="s">
-        <v>190</v>
-      </c>
-      <c r="AE21" s="49">
+      <c r="AB21" s="46"/>
+      <c r="AC21" s="45"/>
+      <c r="AD21" s="45" t="s">
+        <v>186</v>
+      </c>
+      <c r="AE21" s="45">
         <f t="shared" si="0"/>
         <v>17.666666666666668</v>
       </c>
-      <c r="AF21" s="49">
+      <c r="AF21" s="45">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="AG21" s="49"/>
-      <c r="AH21" s="49">
+      <c r="AG21" s="45"/>
+      <c r="AH21" s="45">
         <f t="shared" si="0"/>
         <v>5.5</v>
       </c>
-      <c r="AI21" s="49"/>
-      <c r="AJ21" s="50"/>
-      <c r="AK21" s="50" t="s">
-        <v>191</v>
-      </c>
-      <c r="AL21" s="50">
+      <c r="AI21" s="45"/>
+      <c r="AJ21" s="46"/>
+      <c r="AK21" s="46" t="s">
+        <v>187</v>
+      </c>
+      <c r="AL21" s="46">
         <f t="shared" si="0"/>
         <v>51.571428571428569</v>
       </c>
-      <c r="AM21" s="50">
+      <c r="AM21" s="46">
         <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="AN21" s="50"/>
-      <c r="AO21" s="50">
+      <c r="AN21" s="46"/>
+      <c r="AO21" s="46">
         <f t="shared" si="0"/>
         <v>5.1428571428571432</v>
       </c>
-      <c r="AP21" s="50"/>
-      <c r="AQ21" s="49"/>
-      <c r="AR21" s="49" t="s">
-        <v>191</v>
-      </c>
-      <c r="AS21" s="49">
+      <c r="AP21" s="46"/>
+      <c r="AQ21" s="45"/>
+      <c r="AR21" s="45" t="s">
+        <v>187</v>
+      </c>
+      <c r="AS21" s="45">
         <f t="shared" si="0"/>
         <v>11.857142857142858</v>
       </c>
-      <c r="AT21" s="49">
+      <c r="AT21" s="45">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
-      <c r="AU21" s="49"/>
-      <c r="AV21" s="49">
+      <c r="AU21" s="45"/>
+      <c r="AV21" s="45">
         <f t="shared" si="0"/>
         <v>5.4285714285714288</v>
       </c>
-      <c r="AW21" s="49"/>
-      <c r="AX21" s="32"/>
-      <c r="AY21" s="32">
+      <c r="AW21" s="45"/>
+      <c r="AX21" s="31"/>
+      <c r="AY21" s="31">
         <f t="shared" si="0"/>
         <v>5.8571428571428568</v>
       </c>
-      <c r="AZ21" s="32"/>
-      <c r="BA21" s="55"/>
-      <c r="BB21" s="56"/>
+      <c r="AZ21" s="31"/>
+      <c r="BA21" s="51"/>
+      <c r="BB21" s="52"/>
       <c r="BC21" s="1"/>
       <c r="BD21" s="1"/>
     </row>
-    <row r="22" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:56" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B22" s="1">
         <f>AVERAGE(B12:B20)</f>
         <v>25.666666666666668</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="J22" s="5">
         <f>AVERAGE(J12:J20)</f>
@@ -3997,7 +4007,7 @@
       <c r="N22" s="5"/>
       <c r="O22" s="2"/>
       <c r="P22" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="Q22" s="2">
         <f t="shared" si="1"/>
@@ -4015,7 +4025,7 @@
       <c r="U22" s="2"/>
       <c r="V22" s="5"/>
       <c r="W22" s="5" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="X22" s="5">
         <f t="shared" si="1"/>
@@ -4033,7 +4043,7 @@
       <c r="AB22" s="5"/>
       <c r="AC22" s="2"/>
       <c r="AD22" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="AE22" s="2">
         <f t="shared" si="1"/>
@@ -4051,7 +4061,7 @@
       <c r="AI22" s="2"/>
       <c r="AJ22" s="5"/>
       <c r="AK22" s="5" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="AL22" s="5">
         <f t="shared" si="1"/>
@@ -4069,7 +4079,7 @@
       <c r="AP22" s="5"/>
       <c r="AQ22" s="2"/>
       <c r="AR22" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="AS22" s="2">
         <f t="shared" si="1"/>
@@ -4084,19 +4094,19 @@
         <f t="shared" si="1"/>
         <v>5.666666666666667</v>
       </c>
-      <c r="AW22" s="33"/>
-      <c r="AX22" s="57"/>
-      <c r="AY22" s="57">
+      <c r="AW22" s="32"/>
+      <c r="AX22" s="53"/>
+      <c r="AY22" s="53">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="AZ22" s="58"/>
-      <c r="BA22" s="32"/>
-      <c r="BB22" s="59"/>
+      <c r="AZ22" s="54"/>
+      <c r="BA22" s="31"/>
+      <c r="BB22" s="55"/>
       <c r="BC22" s="1"/>
       <c r="BD22" s="1"/>
     </row>
-    <row r="23" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:56" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -4105,19 +4115,19 @@
         <v>32.9</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="J23" s="5">
         <f>AVERAGE(J2:J20)</f>
@@ -4135,7 +4145,7 @@
       <c r="N23" s="5"/>
       <c r="O23" s="2"/>
       <c r="P23" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="Q23" s="2">
         <f t="shared" si="2"/>
@@ -4153,7 +4163,7 @@
       <c r="U23" s="2"/>
       <c r="V23" s="5"/>
       <c r="W23" s="5" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="X23" s="5">
         <f t="shared" si="2"/>
@@ -4171,7 +4181,7 @@
       <c r="AB23" s="5"/>
       <c r="AC23" s="2"/>
       <c r="AD23" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="AE23" s="2">
         <f t="shared" si="2"/>
@@ -4189,7 +4199,7 @@
       <c r="AI23" s="2"/>
       <c r="AJ23" s="5"/>
       <c r="AK23" s="5" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="AL23" s="5">
         <f t="shared" si="2"/>
@@ -4207,7 +4217,7 @@
       <c r="AP23" s="5"/>
       <c r="AQ23" s="2"/>
       <c r="AR23" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="AS23" s="2">
         <f t="shared" si="2"/>
@@ -4222,19 +4232,19 @@
         <f t="shared" si="2"/>
         <v>5.5</v>
       </c>
-      <c r="AW23" s="33"/>
-      <c r="AX23" s="32"/>
-      <c r="AY23" s="32">
+      <c r="AW23" s="32"/>
+      <c r="AX23" s="31"/>
+      <c r="AY23" s="31">
         <f t="shared" si="2"/>
         <v>5.3</v>
       </c>
-      <c r="AZ23" s="32"/>
-      <c r="BA23" s="60"/>
-      <c r="BB23" s="55"/>
+      <c r="AZ23" s="31"/>
+      <c r="BA23" s="56"/>
+      <c r="BB23" s="51"/>
       <c r="BC23" s="1"/>
       <c r="BD23" s="1"/>
     </row>
-    <row r="24" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -4283,16 +4293,16 @@
       <c r="AT24" s="2"/>
       <c r="AU24" s="2"/>
       <c r="AV24" s="2"/>
-      <c r="AW24" s="33"/>
-      <c r="AX24" s="32"/>
-      <c r="AY24" s="32"/>
-      <c r="AZ24" s="61"/>
-      <c r="BA24" s="62"/>
-      <c r="BB24" s="32"/>
+      <c r="AW24" s="32"/>
+      <c r="AX24" s="31"/>
+      <c r="AY24" s="31"/>
+      <c r="AZ24" s="57"/>
+      <c r="BA24" s="58"/>
+      <c r="BB24" s="31"/>
       <c r="BC24" s="1"/>
       <c r="BD24" s="1"/>
     </row>
-    <row r="25" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -4341,16 +4351,16 @@
       <c r="AT25" s="2"/>
       <c r="AU25" s="2"/>
       <c r="AV25" s="2"/>
-      <c r="AW25" s="33"/>
-      <c r="AX25" s="54"/>
-      <c r="AY25" s="63"/>
-      <c r="AZ25" s="23"/>
-      <c r="BA25" s="43"/>
-      <c r="BB25" s="22"/>
+      <c r="AW25" s="32"/>
+      <c r="AX25" s="50"/>
+      <c r="AY25" s="59"/>
+      <c r="AZ25" s="22"/>
+      <c r="BA25" s="40"/>
+      <c r="BB25" s="21"/>
       <c r="BC25" s="1"/>
       <c r="BD25" s="1"/>
     </row>
-    <row r="26" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:56" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
@@ -4402,15 +4412,15 @@
       <c r="AU26" s="2"/>
       <c r="AV26" s="2"/>
       <c r="AW26" s="2"/>
-      <c r="AX26" s="36"/>
-      <c r="AY26" s="36"/>
-      <c r="AZ26" s="36"/>
-      <c r="BA26" s="36"/>
-      <c r="BB26" s="36"/>
+      <c r="AX26" s="35"/>
+      <c r="AY26" s="35"/>
+      <c r="AZ26" s="35"/>
+      <c r="BA26" s="35"/>
+      <c r="BB26" s="35"/>
       <c r="BC26" s="1"/>
       <c r="BD26" s="1"/>
     </row>
-    <row r="27" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -4466,7 +4476,7 @@
       <c r="BC27" s="1"/>
       <c r="BD27" s="1"/>
     </row>
-    <row r="28" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -4522,7 +4532,7 @@
       <c r="BC28" s="1"/>
       <c r="BD28" s="1"/>
     </row>
-    <row r="29" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -4578,7 +4588,7 @@
       <c r="BC29" s="1"/>
       <c r="BD29" s="1"/>
     </row>
-    <row r="30" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -4634,7 +4644,7 @@
       <c r="BC30" s="1"/>
       <c r="BD30" s="1"/>
     </row>
-    <row r="31" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -4690,7 +4700,7 @@
       <c r="BC31" s="1"/>
       <c r="BD31" s="1"/>
     </row>
-    <row r="32" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -4746,7 +4756,7 @@
       <c r="BC32" s="1"/>
       <c r="BD32" s="1"/>
     </row>
-    <row r="33" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -4802,7 +4812,7 @@
       <c r="BC33" s="1"/>
       <c r="BD33" s="1"/>
     </row>
-    <row r="34" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -4858,7 +4868,7 @@
       <c r="BC34" s="1"/>
       <c r="BD34" s="1"/>
     </row>
-    <row r="35" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -4914,7 +4924,7 @@
       <c r="BC35" s="1"/>
       <c r="BD35" s="1"/>
     </row>
-    <row r="36" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -4970,7 +4980,7 @@
       <c r="BC36" s="1"/>
       <c r="BD36" s="1"/>
     </row>
-    <row r="37" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -5026,7 +5036,7 @@
       <c r="BC37" s="1"/>
       <c r="BD37" s="1"/>
     </row>
-    <row r="38" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -5082,7 +5092,7 @@
       <c r="BC38" s="1"/>
       <c r="BD38" s="1"/>
     </row>
-    <row r="39" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -5138,7 +5148,7 @@
       <c r="BC39" s="1"/>
       <c r="BD39" s="1"/>
     </row>
-    <row r="40" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -5194,7 +5204,7 @@
       <c r="BC40" s="1"/>
       <c r="BD40" s="1"/>
     </row>
-    <row r="41" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -5250,7 +5260,7 @@
       <c r="BC41" s="1"/>
       <c r="BD41" s="1"/>
     </row>
-    <row r="42" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -5306,7 +5316,7 @@
       <c r="BC42" s="1"/>
       <c r="BD42" s="1"/>
     </row>
-    <row r="43" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -5362,7 +5372,7 @@
       <c r="BC43" s="1"/>
       <c r="BD43" s="1"/>
     </row>
-    <row r="44" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -5418,7 +5428,7 @@
       <c r="BC44" s="1"/>
       <c r="BD44" s="1"/>
     </row>
-    <row r="45" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -5474,7 +5484,7 @@
       <c r="BC45" s="1"/>
       <c r="BD45" s="1"/>
     </row>
-    <row r="46" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -5530,7 +5540,7 @@
       <c r="BC46" s="1"/>
       <c r="BD46" s="1"/>
     </row>
-    <row r="47" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -5586,7 +5596,7 @@
       <c r="BC47" s="1"/>
       <c r="BD47" s="1"/>
     </row>
-    <row r="48" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -5642,7 +5652,7 @@
       <c r="BC48" s="1"/>
       <c r="BD48" s="1"/>
     </row>
-    <row r="49" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -5698,7 +5708,7 @@
       <c r="BC49" s="1"/>
       <c r="BD49" s="1"/>
     </row>
-    <row r="50" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -5754,7 +5764,7 @@
       <c r="BC50" s="1"/>
       <c r="BD50" s="1"/>
     </row>
-    <row r="51" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -5810,7 +5820,7 @@
       <c r="BC51" s="1"/>
       <c r="BD51" s="1"/>
     </row>
-    <row r="52" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -5866,7 +5876,7 @@
       <c r="BC52" s="1"/>
       <c r="BD52" s="1"/>
     </row>
-    <row r="53" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
     </row>
   </sheetData>

</xml_diff>